<commit_message>
Deploying to gh-pages from  @ 8f97e80b6508254100d88653f09e4426c15e2fd7 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/15.3.1.1.xlsx
+++ b/en/downloads/data-excel/15.3.1.1.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <t>15.3.1.1. Площадь пашни по причинам неиспользования</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -32,9 +29,6 @@
   </si>
   <si>
     <t>Площадь неиспользованной пашни</t>
-  </si>
-  <si>
-    <t>15.3.1.1. Пайдаланбаган себептер боюнча айдоо аянты</t>
   </si>
   <si>
     <t>Бардыгы</t>
@@ -107,22 +101,40 @@
     <t>(at beginning of year, thousand hectares)</t>
   </si>
   <si>
-    <t>Экономическая нецелесообразность</t>
-  </si>
-  <si>
     <t>Другие причины (под промышленность, расширения населенных пунктов и другие)</t>
   </si>
   <si>
-    <t>Economic inexpediency</t>
-  </si>
-  <si>
     <t>Other reasons (for industry, expansion of settlements and others)</t>
   </si>
   <si>
-    <t>Экономикалык максатка ылайыксыздык</t>
-  </si>
-  <si>
     <t>Башка себептер (өнөр жай, калктуу конуштарды кеңейтүү жана башкалар)</t>
+  </si>
+  <si>
+    <t>15.3.1.1 Пайдаланбаган себептер боюнча айдоо аянты</t>
+  </si>
+  <si>
+    <t>15.3.1.1 Площадь пашни по причинам неиспользования</t>
+  </si>
+  <si>
+    <t>Катуу жаанчыл (жазында топуракта нымдуулуктун жетишсиздиги)</t>
+  </si>
+  <si>
+    <t>Жесткая богара (недостаток количества влаги в почве весной)</t>
+  </si>
+  <si>
+    <t>Hard rainfed (lack of moisture in the soil in spring)</t>
+  </si>
+  <si>
+    <t>1 280,6</t>
+  </si>
+  <si>
+    <t>1 287,9</t>
+  </si>
+  <si>
+    <t>1 287,8</t>
+  </si>
+  <si>
+    <t>1 287,6</t>
   </si>
 </sst>
 </file>
@@ -234,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
@@ -276,16 +288,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -592,9 +610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
@@ -604,38 +624,38 @@
     <col min="10" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27.75" customHeight="1">
+    <row r="1" spans="1:11" ht="27.75" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="12.75" thickBot="1"/>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="12.75" thickBot="1"/>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="D4" s="4">
         <v>2015</v>
@@ -658,31 +678,34 @@
       <c r="J4" s="4">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1">
+      <c r="K4" s="4">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="14">
-        <v>1280.5999999999999</v>
+        <v>12</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="E5" s="14">
         <v>1280.5999999999999</v>
       </c>
-      <c r="F5" s="14">
-        <v>1287.9000000000001</v>
-      </c>
-      <c r="G5" s="14">
-        <v>1287.8</v>
-      </c>
-      <c r="H5" s="14">
-        <v>1287.5999999999999</v>
+      <c r="F5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="I5" s="14">
         <v>1287.4000000000001</v>
@@ -690,247 +713,272 @@
       <c r="J5" s="14">
         <v>1287.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1">
+      <c r="K5" s="19">
+        <v>1286.4000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.25" customHeight="1">
       <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="16">
+        <v>89.2</v>
+      </c>
+      <c r="E6" s="16">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="F6" s="16">
+        <v>74</v>
+      </c>
+      <c r="G6" s="16">
+        <v>66.5</v>
+      </c>
+      <c r="H6" s="16">
+        <v>62.5</v>
+      </c>
+      <c r="I6" s="16">
+        <v>55.8</v>
+      </c>
+      <c r="J6" s="16">
+        <v>52.9</v>
+      </c>
+      <c r="K6" s="15">
+        <v>48.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="16">
+        <v>5</v>
+      </c>
+      <c r="E8" s="16">
+        <v>3.8</v>
+      </c>
+      <c r="F8" s="16">
+        <v>3.3</v>
+      </c>
+      <c r="G8" s="16">
+        <v>3.1</v>
+      </c>
+      <c r="H8" s="16">
+        <v>2.8</v>
+      </c>
+      <c r="I8" s="16">
+        <v>2.5</v>
+      </c>
+      <c r="J8" s="16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K8" s="15">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="25.5" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="15">
-        <v>90</v>
-      </c>
-      <c r="E6" s="15">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="F6" s="15">
-        <v>74.8</v>
-      </c>
-      <c r="G6" s="15">
-        <v>67.3</v>
-      </c>
-      <c r="H6" s="15">
-        <v>63.3</v>
-      </c>
-      <c r="I6" s="15">
-        <v>56.6</v>
-      </c>
-      <c r="J6" s="15">
-        <v>53.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="D9" s="16">
+        <v>13.6</v>
+      </c>
+      <c r="E9" s="16">
+        <v>13.8</v>
+      </c>
+      <c r="F9" s="16">
+        <v>11.7</v>
+      </c>
+      <c r="G9" s="16">
+        <v>11.6</v>
+      </c>
+      <c r="H9" s="16">
+        <v>11.1</v>
+      </c>
+      <c r="I9" s="16">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J9" s="16">
+        <v>8.4</v>
+      </c>
+      <c r="K9" s="15">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="25.5" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="15">
-        <v>5</v>
-      </c>
-      <c r="E8" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="F8" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="G8" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="H8" s="15">
-        <v>2.8</v>
-      </c>
-      <c r="I8" s="15">
-        <v>2.5</v>
-      </c>
-      <c r="J8" s="15">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="25.5" customHeight="1">
-      <c r="A9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="D10" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="F10" s="17">
+        <v>1.04</v>
+      </c>
+      <c r="G10" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="24.75" customHeight="1">
+      <c r="A11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="16">
+        <v>44.4</v>
+      </c>
+      <c r="E11" s="16">
+        <v>40.1</v>
+      </c>
+      <c r="F11" s="16">
+        <v>36.4</v>
+      </c>
+      <c r="G11" s="16">
+        <v>31.4</v>
+      </c>
+      <c r="H11" s="16">
+        <v>31.7</v>
+      </c>
+      <c r="I11" s="16">
+        <v>27.2</v>
+      </c>
+      <c r="J11" s="16">
+        <v>26.2</v>
+      </c>
+      <c r="K11" s="15">
         <v>22</v>
       </c>
-      <c r="D9" s="15">
-        <v>13.8</v>
-      </c>
-      <c r="E9" s="15">
-        <v>14</v>
-      </c>
-      <c r="F9" s="15">
-        <v>12</v>
-      </c>
-      <c r="G9" s="15">
-        <v>11.8</v>
-      </c>
-      <c r="H9" s="15">
-        <v>11.1</v>
-      </c>
-      <c r="I9" s="15">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J9" s="15">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="25.5" customHeight="1">
-      <c r="A10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="13" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="14.25" customHeight="1">
+      <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="16">
-        <v>0.4</v>
-      </c>
-      <c r="E10" s="16">
-        <v>0.4</v>
-      </c>
-      <c r="F10" s="16">
-        <v>1.04</v>
-      </c>
-      <c r="G10" s="16">
-        <v>1.6</v>
-      </c>
-      <c r="H10" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I10" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="J10" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="16">
+        <v>16.5</v>
+      </c>
+      <c r="E12" s="16">
+        <v>15.1</v>
+      </c>
+      <c r="F12" s="16">
+        <v>13.7</v>
+      </c>
+      <c r="G12" s="16">
+        <v>11.9</v>
+      </c>
+      <c r="H12" s="16">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I12" s="16">
+        <v>9.4</v>
+      </c>
+      <c r="J12" s="16">
+        <v>8.4</v>
+      </c>
+      <c r="K12" s="15">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="24.75" thickBot="1">
+      <c r="A13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="15">
-        <v>44.4</v>
-      </c>
-      <c r="E11" s="15">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="F11" s="15">
-        <v>36.5</v>
-      </c>
-      <c r="G11" s="15">
-        <v>31.5</v>
-      </c>
-      <c r="H11" s="15">
-        <v>31.7</v>
-      </c>
-      <c r="I11" s="15">
-        <v>27.2</v>
-      </c>
-      <c r="J11" s="15">
-        <v>26.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="15">
-        <v>16.5</v>
-      </c>
-      <c r="E12" s="15">
-        <v>15.1</v>
-      </c>
-      <c r="F12" s="15">
-        <v>13.7</v>
-      </c>
-      <c r="G12" s="15">
-        <v>11.6</v>
-      </c>
-      <c r="H12" s="15">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="I12" s="15">
-        <v>9.4</v>
-      </c>
-      <c r="J12" s="15">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="24.75" thickBot="1">
-      <c r="A13" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="B13" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="17">
-        <v>9.8999999999999986</v>
-      </c>
-      <c r="E13" s="17">
-        <v>8.4000000000000075</v>
-      </c>
-      <c r="F13" s="17">
-        <v>8.2600000000000016</v>
-      </c>
-      <c r="G13" s="17">
-        <v>7.7000000000000046</v>
-      </c>
-      <c r="H13" s="17">
-        <v>7</v>
-      </c>
-      <c r="I13" s="17">
-        <v>7.2999999999999989</v>
-      </c>
-      <c r="J13" s="17">
-        <v>7.4</v>
+        <v>29</v>
+      </c>
+      <c r="D13" s="18">
+        <v>9.3000000000000043</v>
+      </c>
+      <c r="E13" s="18">
+        <v>7.9</v>
+      </c>
+      <c r="F13" s="18">
+        <v>7.860000000000003</v>
+      </c>
+      <c r="G13" s="18">
+        <v>6.9999999999999982</v>
+      </c>
+      <c r="H13" s="18">
+        <v>6.2000000000000028</v>
+      </c>
+      <c r="I13" s="18">
+        <v>6.5000000000000018</v>
+      </c>
+      <c r="J13" s="18">
+        <v>6.6999999999999975</v>
+      </c>
+      <c r="K13" s="18">
+        <v>9.7999999999999936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>